<commit_message>
Add Item and Item's feature
Creating item@index function
</commit_message>
<xml_diff>
--- a/Routing Table.xlsx
+++ b/Routing Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0 - Web Based Development\0 - Laravel Projects\x-market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{36DECF6E-B4AD-445C-8BF5-FFE5F23714D2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3378B2A8-FF3F-41A7-A740-CDAE73600496}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5652" xr2:uid="{43463EAA-A319-4CAD-BB61-1CA437DD593E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
   <si>
     <t>Users</t>
   </si>
@@ -243,12 +243,6 @@
     <t>user.profile.update</t>
   </si>
   <si>
-    <t>profile.show</t>
-  </si>
-  <si>
-    <t>profile.edit</t>
-  </si>
-  <si>
     <t>transaction.show</t>
   </si>
   <si>
@@ -258,7 +252,97 @@
     <t>Users/{Username}</t>
   </si>
   <si>
-    <t>Users/{Username}/Update</t>
+    <t>users.index</t>
+  </si>
+  <si>
+    <t>users.login</t>
+  </si>
+  <si>
+    <t>users.register</t>
+  </si>
+  <si>
+    <t>profiles.show</t>
+  </si>
+  <si>
+    <t>profiles.edit</t>
+  </si>
+  <si>
+    <t>Users/{Username}/edit</t>
+  </si>
+  <si>
+    <t>item.show</t>
+  </si>
+  <si>
+    <t>item.create</t>
+  </si>
+  <si>
+    <t>item.store</t>
+  </si>
+  <si>
+    <t>item.edit</t>
+  </si>
+  <si>
+    <t>item.delete</t>
+  </si>
+  <si>
+    <t>item.buy</t>
+  </si>
+  <si>
+    <t>item.update</t>
+  </si>
+  <si>
+    <t>item.destroy</t>
+  </si>
+  <si>
+    <t>item.transaction.add</t>
+  </si>
+  <si>
+    <t>items.show</t>
+  </si>
+  <si>
+    <t>items.create</t>
+  </si>
+  <si>
+    <t>items.edit</t>
+  </si>
+  <si>
+    <t>items.delete</t>
+  </si>
+  <si>
+    <t>items.buy</t>
+  </si>
+  <si>
+    <t>service.index</t>
+  </si>
+  <si>
+    <t>service.show</t>
+  </si>
+  <si>
+    <t>category.index</t>
+  </si>
+  <si>
+    <t>category.show</t>
+  </si>
+  <si>
+    <t>category.subcategory.show</t>
+  </si>
+  <si>
+    <t>services.index</t>
+  </si>
+  <si>
+    <t>services.show</t>
+  </si>
+  <si>
+    <t>search.engine</t>
+  </si>
+  <si>
+    <t>Items/{Username}/{ItemID}</t>
+  </si>
+  <si>
+    <t>item.index</t>
+  </si>
+  <si>
+    <t>items.index</t>
   </si>
 </sst>
 </file>
@@ -674,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AD5C87-9DF7-45EE-84EB-1044C9ED29C4}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,7 +824,7 @@
         <v>60</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -764,7 +848,7 @@
         <v>61</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -826,7 +910,7 @@
         <v>65</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -855,7 +939,7 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>49</v>
@@ -871,7 +955,7 @@
         <v>67</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -879,7 +963,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>49</v>
@@ -897,7 +981,7 @@
         <v>69</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -905,7 +989,7 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>49</v>
@@ -944,7 +1028,7 @@
         <v>70</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -970,7 +1054,7 @@
         <v>68</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -984,7 +1068,7 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>49</v>
@@ -996,7 +1080,12 @@
       <c r="F15" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1015,9 +1104,14 @@
       <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1030,13 +1124,20 @@
       <c r="D17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F17" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1051,9 +1152,12 @@
       <c r="F18" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1072,9 +1176,14 @@
       <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1091,9 +1200,12 @@
       <c r="F20" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1112,9 +1224,14 @@
       <c r="F21" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G21" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1131,9 +1248,12 @@
       <c r="F22" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1152,9 +1272,14 @@
       <c r="F23" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1170,12 +1295,15 @@
       <c r="F24" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1192,9 +1320,14 @@
       <c r="F26" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1211,15 +1344,20 @@
       <c r="F27" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1236,9 +1374,11 @@
       <c r="F29" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G29" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1255,9 +1395,11 @@
       <c r="F30" t="s">
         <v>27</v>
       </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1274,9 +1416,11 @@
       <c r="F31" t="s">
         <v>29</v>
       </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G31" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1327,7 +1471,9 @@
       <c r="F35" t="s">
         <v>34</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>

</xml_diff>

<commit_message>
Added Category and SubCategory
</commit_message>
<xml_diff>
--- a/Routing Table.xlsx
+++ b/Routing Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0 - Web Based Development\0 - Laravel Projects\x-market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9CD36C52-7CB1-4F28-8F44-315BF088B3CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AE2DA2CD-A62D-43CA-A396-79AD8534D1DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5652" xr2:uid="{43463EAA-A319-4CAD-BB61-1CA437DD593E}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AD5C87-9DF7-45EE-84EB-1044C9ED29C4}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,7 +928,7 @@
       <c r="G3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       <c r="G9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1083,7 +1083,7 @@
       <c r="G10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="3" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merge Backend with Frontend
</commit_message>
<xml_diff>
--- a/Routing Table.xlsx
+++ b/Routing Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0 - Web Based Development\0 - Laravel Projects\x-market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AE2DA2CD-A62D-43CA-A396-79AD8534D1DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FC6A80B0-079C-4184-8D31-3A4FCB913EE9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5652" xr2:uid="{43463EAA-A319-4CAD-BB61-1CA437DD593E}"/>
   </bookViews>
@@ -514,7 +514,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -543,6 +543,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
@@ -863,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AD5C87-9DF7-45EE-84EB-1044C9ED29C4}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,7 +1425,7 @@
       <c r="F26" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>95</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -1446,7 +1449,7 @@
       <c r="F27" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="4" t="s">
         <v>96</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -1472,7 +1475,7 @@
       <c r="F28" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="4" t="s">
         <v>108</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -1496,7 +1499,7 @@
       <c r="F29" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="4" t="s">
         <v>113</v>
       </c>
       <c r="H29" s="11"/>
@@ -1520,7 +1523,7 @@
       <c r="F30" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H30" s="4" t="s">
@@ -1544,7 +1547,7 @@
       <c r="F31" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="4" t="s">
         <v>115</v>
       </c>
       <c r="H31" s="11"/>
@@ -1568,7 +1571,7 @@
       <c r="F32" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H32" s="4" t="s">
@@ -1590,7 +1593,7 @@
       <c r="F33" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="4" t="s">
         <v>121</v>
       </c>
       <c r="H33" s="11"/>
@@ -1612,10 +1615,10 @@
       <c r="F35" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="12" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1636,10 +1639,10 @@
       <c r="F36" t="s">
         <v>27</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="12" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1660,10 +1663,10 @@
       <c r="F37" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="12" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1686,10 +1689,10 @@
       <c r="F38" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="12" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1710,7 +1713,7 @@
       <c r="F39" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="5" t="s">
         <v>129</v>
       </c>
       <c r="H39" s="11"/>
@@ -1732,7 +1735,7 @@
       <c r="F40" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="5" t="s">
         <v>130</v>
       </c>
       <c r="H40" s="11"/>
@@ -1754,7 +1757,7 @@
       <c r="F41" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="5" t="s">
         <v>131</v>
       </c>
       <c r="H41" s="11"/>

</xml_diff>